<commit_message>
Updated with sample 24
</commit_message>
<xml_diff>
--- a/Lab/LabJournal.xlsx
+++ b/Lab/LabJournal.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="83">
   <si>
     <t>Laboratory Journal</t>
   </si>
@@ -336,7 +336,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -367,6 +367,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="42">
     <border>
@@ -860,7 +866,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="141">
+  <cellXfs count="142">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -974,6 +980,204 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -989,8 +1193,65 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1019,259 +1280,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="31" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="23" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="41" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1576,15 +1585,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="33" x14ac:dyDescent="0.35">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="108" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
+      <c r="D2" s="108"/>
+      <c r="E2" s="108"/>
+      <c r="F2" s="108"/>
+      <c r="G2" s="108"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4" s="3" t="s">
@@ -1624,29 +1633,29 @@
       <c r="G6" s="4"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B8" s="43" t="s">
+      <c r="B8" s="109" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="43"/>
+      <c r="C8" s="109"/>
       <c r="D8" s="7"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:7" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="110" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="44"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
+      <c r="C9" s="110"/>
+      <c r="D9" s="110"/>
+      <c r="E9" s="110"/>
+      <c r="F9" s="110"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B10" s="45"/>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="45"/>
-      <c r="F10" s="45"/>
+      <c r="B10" s="111"/>
+      <c r="C10" s="111"/>
+      <c r="D10" s="111"/>
+      <c r="E10" s="111"/>
+      <c r="F10" s="111"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B11" s="11"/>
@@ -1681,7 +1690,7 @@
       <c r="E13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F13" s="41" t="s">
+      <c r="F13" s="107" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1696,7 +1705,7 @@
       <c r="E14" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="F14" s="41"/>
+      <c r="F14" s="107"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
@@ -1711,19 +1720,19 @@
       <c r="E15" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="41"/>
+      <c r="F15" s="107"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
-      <c r="F16" s="41"/>
+      <c r="F16" s="107"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
-      <c r="F17" s="41"/>
+      <c r="F17" s="107"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
@@ -1734,7 +1743,7 @@
       </c>
       <c r="D18" s="5"/>
       <c r="E18" s="5"/>
-      <c r="F18" s="41"/>
+      <c r="F18" s="107"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
       <c r="F19" s="14"/>
@@ -1766,1356 +1775,1381 @@
   <dimension ref="B1:W33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O37" sqref="O37"/>
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.83203125" style="93" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="93"/>
-    <col min="3" max="3" width="2.5" style="93" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="98"/>
-    <col min="5" max="6" width="10.83203125" style="93"/>
-    <col min="7" max="7" width="12.1640625" style="93" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="10.83203125" style="93"/>
-    <col min="11" max="12" width="10.83203125" style="93" customWidth="1"/>
-    <col min="13" max="14" width="10.83203125" style="106"/>
-    <col min="15" max="15" width="10.83203125" style="93" customWidth="1"/>
-    <col min="16" max="16" width="10.83203125" style="106" customWidth="1"/>
-    <col min="17" max="17" width="10.83203125" style="93" customWidth="1"/>
-    <col min="18" max="21" width="10.83203125" style="93"/>
-    <col min="22" max="22" width="10.83203125" style="106"/>
-    <col min="23" max="23" width="47.83203125" style="106" customWidth="1"/>
-    <col min="24" max="16384" width="10.83203125" style="93"/>
+    <col min="1" max="1" width="2.83203125" style="71" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="71"/>
+    <col min="3" max="3" width="2.5" style="71" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="76"/>
+    <col min="5" max="6" width="10.83203125" style="71"/>
+    <col min="7" max="7" width="12.1640625" style="71" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="10.83203125" style="71"/>
+    <col min="11" max="12" width="10.83203125" style="71" customWidth="1"/>
+    <col min="13" max="14" width="10.83203125" style="81"/>
+    <col min="15" max="15" width="10.83203125" style="71" customWidth="1"/>
+    <col min="16" max="16" width="10.83203125" style="81" customWidth="1"/>
+    <col min="17" max="17" width="10.83203125" style="71" customWidth="1"/>
+    <col min="18" max="21" width="10.83203125" style="71"/>
+    <col min="22" max="22" width="10.83203125" style="81"/>
+    <col min="23" max="23" width="47.83203125" style="81" customWidth="1"/>
+    <col min="24" max="16384" width="10.83203125" style="71"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B2" s="119" t="s">
+      <c r="B2" s="121" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="120"/>
-      <c r="D2" s="121" t="s">
+      <c r="C2" s="114"/>
+      <c r="D2" s="118" t="s">
         <v>82</v>
       </c>
-      <c r="E2" s="122"/>
-      <c r="F2" s="122"/>
-      <c r="G2" s="122"/>
-      <c r="H2" s="122"/>
-      <c r="I2" s="122"/>
-      <c r="J2" s="122"/>
-      <c r="K2" s="122"/>
-      <c r="L2" s="122"/>
-      <c r="M2" s="123"/>
-      <c r="N2" s="124" t="s">
+      <c r="E2" s="119"/>
+      <c r="F2" s="119"/>
+      <c r="G2" s="119"/>
+      <c r="H2" s="119"/>
+      <c r="I2" s="119"/>
+      <c r="J2" s="119"/>
+      <c r="K2" s="119"/>
+      <c r="L2" s="119"/>
+      <c r="M2" s="120"/>
+      <c r="N2" s="112" t="s">
         <v>44</v>
       </c>
-      <c r="O2" s="125"/>
-      <c r="P2" s="120"/>
-      <c r="Q2" s="124" t="s">
+      <c r="O2" s="113"/>
+      <c r="P2" s="114"/>
+      <c r="Q2" s="112" t="s">
         <v>48</v>
       </c>
-      <c r="R2" s="125"/>
-      <c r="S2" s="125"/>
-      <c r="T2" s="125"/>
-      <c r="U2" s="125"/>
-      <c r="V2" s="120"/>
-      <c r="W2" s="126" t="s">
+      <c r="R2" s="113"/>
+      <c r="S2" s="113"/>
+      <c r="T2" s="113"/>
+      <c r="U2" s="113"/>
+      <c r="V2" s="114"/>
+      <c r="W2" s="93" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="3" spans="2:23" ht="32" x14ac:dyDescent="0.2">
-      <c r="B3" s="127"/>
-      <c r="C3" s="118"/>
-      <c r="D3" s="96" t="s">
+      <c r="B3" s="122"/>
+      <c r="C3" s="123"/>
+      <c r="D3" s="74" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="95" t="s">
+      <c r="E3" s="73" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="95" t="s">
+      <c r="F3" s="73" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="95" t="s">
+      <c r="G3" s="73" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="95" t="s">
+      <c r="H3" s="73" t="s">
         <v>30</v>
       </c>
-      <c r="I3" s="95" t="s">
+      <c r="I3" s="73" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="95" t="s">
+      <c r="J3" s="73" t="s">
         <v>28</v>
       </c>
-      <c r="K3" s="97" t="s">
+      <c r="K3" s="75" t="s">
         <v>56</v>
       </c>
-      <c r="L3" s="97" t="s">
+      <c r="L3" s="75" t="s">
         <v>79</v>
       </c>
-      <c r="M3" s="95" t="s">
+      <c r="M3" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="N3" s="95" t="s">
+      <c r="N3" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="O3" s="95" t="s">
+      <c r="O3" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="P3" s="95" t="s">
+      <c r="P3" s="73" t="s">
         <v>47</v>
       </c>
-      <c r="Q3" s="95" t="s">
+      <c r="Q3" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="R3" s="95" t="s">
+      <c r="R3" s="73" t="s">
         <v>43</v>
       </c>
-      <c r="S3" s="95"/>
-      <c r="T3" s="95"/>
-      <c r="U3" s="107"/>
-      <c r="V3" s="95"/>
-      <c r="W3" s="128"/>
+      <c r="S3" s="73"/>
+      <c r="T3" s="73"/>
+      <c r="U3" s="82"/>
+      <c r="V3" s="73"/>
+      <c r="W3" s="94"/>
     </row>
     <row r="4" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B4" s="129">
+      <c r="B4" s="95">
         <v>1</v>
       </c>
-      <c r="C4" s="130"/>
-      <c r="D4" s="114">
+      <c r="C4" s="96"/>
+      <c r="D4" s="89">
         <v>42775</v>
       </c>
-      <c r="E4" s="106" t="s">
+      <c r="E4" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="106">
+      <c r="F4" s="81">
         <v>-0.1</v>
       </c>
-      <c r="G4" s="106" t="s">
+      <c r="G4" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="H4" s="106">
+      <c r="H4" s="81">
         <v>120</v>
       </c>
-      <c r="I4" s="106">
+      <c r="I4" s="81">
         <v>12</v>
       </c>
-      <c r="J4" s="106" t="s">
+      <c r="J4" s="81" t="s">
         <v>31</v>
       </c>
-      <c r="K4" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="L4" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="M4" s="101" t="s">
+      <c r="K4" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="L4" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="M4" s="79" t="s">
         <v>33</v>
       </c>
-      <c r="N4" s="109">
+      <c r="N4" s="84">
         <v>1</v>
       </c>
-      <c r="O4" s="106"/>
-      <c r="P4" s="101"/>
-      <c r="Q4" s="106"/>
-      <c r="R4" s="106"/>
-      <c r="S4" s="106"/>
-      <c r="T4" s="106"/>
-      <c r="U4" s="106"/>
-      <c r="V4" s="99"/>
-      <c r="W4" s="131"/>
+      <c r="O4" s="81"/>
+      <c r="P4" s="79"/>
+      <c r="Q4" s="81"/>
+      <c r="R4" s="81"/>
+      <c r="S4" s="81"/>
+      <c r="T4" s="81"/>
+      <c r="U4" s="81"/>
+      <c r="V4" s="77"/>
+      <c r="W4" s="97"/>
     </row>
     <row r="5" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B5" s="129">
+      <c r="B5" s="95">
         <v>2</v>
       </c>
-      <c r="C5" s="130"/>
-      <c r="D5" s="115">
+      <c r="C5" s="96"/>
+      <c r="D5" s="90">
         <v>42776</v>
       </c>
-      <c r="E5" s="106" t="s">
+      <c r="E5" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="106">
+      <c r="F5" s="81">
         <v>-0.1</v>
       </c>
-      <c r="G5" s="106" t="s">
+      <c r="G5" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="106">
+      <c r="H5" s="81">
         <v>180</v>
       </c>
-      <c r="I5" s="106">
+      <c r="I5" s="81">
         <v>12</v>
       </c>
-      <c r="J5" s="106">
+      <c r="J5" s="81">
         <v>28</v>
       </c>
-      <c r="K5" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="L5" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="M5" s="99" t="s">
-        <v>34</v>
-      </c>
-      <c r="N5" s="110">
+      <c r="K5" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="L5" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="M5" s="77" t="s">
+        <v>34</v>
+      </c>
+      <c r="N5" s="85">
         <v>1</v>
       </c>
-      <c r="O5" s="106"/>
-      <c r="P5" s="99"/>
-      <c r="Q5" s="106"/>
-      <c r="R5" s="106"/>
-      <c r="S5" s="106"/>
-      <c r="T5" s="106"/>
-      <c r="U5" s="106"/>
-      <c r="V5" s="99"/>
-      <c r="W5" s="131"/>
+      <c r="O5" s="81"/>
+      <c r="P5" s="77"/>
+      <c r="Q5" s="81"/>
+      <c r="R5" s="81"/>
+      <c r="S5" s="81"/>
+      <c r="T5" s="81"/>
+      <c r="U5" s="81"/>
+      <c r="V5" s="77"/>
+      <c r="W5" s="97"/>
     </row>
     <row r="6" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B6" s="129">
+      <c r="B6" s="95">
         <v>3</v>
       </c>
-      <c r="C6" s="130"/>
-      <c r="D6" s="115">
+      <c r="C6" s="96"/>
+      <c r="D6" s="90">
         <v>42788</v>
       </c>
-      <c r="E6" s="106" t="s">
+      <c r="E6" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="F6" s="106">
+      <c r="F6" s="81">
         <v>-0.1</v>
       </c>
-      <c r="G6" s="106" t="s">
+      <c r="G6" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="106">
+      <c r="H6" s="81">
         <v>180</v>
       </c>
-      <c r="I6" s="106">
+      <c r="I6" s="81">
         <v>12</v>
       </c>
-      <c r="J6" s="106">
+      <c r="J6" s="81">
         <v>28</v>
       </c>
-      <c r="K6" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="L6" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="M6" s="99" t="s">
-        <v>34</v>
-      </c>
-      <c r="N6" s="110">
+      <c r="K6" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" s="77" t="s">
+        <v>34</v>
+      </c>
+      <c r="N6" s="85">
         <v>1</v>
       </c>
-      <c r="O6" s="106"/>
-      <c r="P6" s="99"/>
-      <c r="Q6" s="106"/>
-      <c r="R6" s="106"/>
-      <c r="S6" s="106"/>
-      <c r="T6" s="106"/>
-      <c r="U6" s="106"/>
-      <c r="V6" s="99"/>
-      <c r="W6" s="131"/>
+      <c r="O6" s="81"/>
+      <c r="P6" s="77"/>
+      <c r="Q6" s="81"/>
+      <c r="R6" s="81"/>
+      <c r="S6" s="81"/>
+      <c r="T6" s="81"/>
+      <c r="U6" s="81"/>
+      <c r="V6" s="77"/>
+      <c r="W6" s="97"/>
     </row>
     <row r="7" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B7" s="129">
+      <c r="B7" s="95">
         <v>4</v>
       </c>
-      <c r="C7" s="130"/>
-      <c r="D7" s="115">
+      <c r="C7" s="96"/>
+      <c r="D7" s="90">
         <v>42788</v>
       </c>
-      <c r="E7" s="106" t="s">
+      <c r="E7" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="106">
+      <c r="F7" s="81">
         <v>-0.1</v>
       </c>
-      <c r="G7" s="106" t="s">
+      <c r="G7" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="H7" s="106">
+      <c r="H7" s="81">
         <v>180</v>
       </c>
-      <c r="I7" s="106">
+      <c r="I7" s="81">
         <v>12</v>
       </c>
-      <c r="J7" s="106">
+      <c r="J7" s="81">
         <v>28</v>
       </c>
-      <c r="K7" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="L7" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="M7" s="99" t="s">
-        <v>34</v>
-      </c>
-      <c r="N7" s="110">
+      <c r="K7" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" s="77" t="s">
+        <v>34</v>
+      </c>
+      <c r="N7" s="85">
         <v>1</v>
       </c>
-      <c r="O7" s="106"/>
-      <c r="P7" s="99"/>
-      <c r="Q7" s="106"/>
-      <c r="R7" s="106"/>
-      <c r="S7" s="106"/>
-      <c r="T7" s="106"/>
-      <c r="U7" s="106"/>
-      <c r="V7" s="99"/>
-      <c r="W7" s="131"/>
+      <c r="O7" s="81"/>
+      <c r="P7" s="77"/>
+      <c r="Q7" s="81"/>
+      <c r="R7" s="81"/>
+      <c r="S7" s="81"/>
+      <c r="T7" s="81"/>
+      <c r="U7" s="81"/>
+      <c r="V7" s="77"/>
+      <c r="W7" s="97"/>
     </row>
     <row r="8" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B8" s="129">
+      <c r="B8" s="95">
         <v>5</v>
       </c>
-      <c r="C8" s="130"/>
-      <c r="D8" s="115">
+      <c r="C8" s="96"/>
+      <c r="D8" s="90">
         <v>42790</v>
       </c>
-      <c r="E8" s="106" t="s">
+      <c r="E8" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="F8" s="106">
+      <c r="F8" s="81">
         <v>-0.1</v>
       </c>
-      <c r="G8" s="106" t="s">
+      <c r="G8" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="H8" s="106">
+      <c r="H8" s="81">
         <v>180</v>
       </c>
-      <c r="I8" s="106">
+      <c r="I8" s="81">
         <v>12</v>
       </c>
-      <c r="J8" s="106">
+      <c r="J8" s="81">
         <v>60</v>
       </c>
-      <c r="K8" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="L8" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="M8" s="99" t="s">
-        <v>34</v>
-      </c>
-      <c r="N8" s="110">
+      <c r="K8" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="M8" s="77" t="s">
+        <v>34</v>
+      </c>
+      <c r="N8" s="85">
         <v>1</v>
       </c>
-      <c r="O8" s="106"/>
-      <c r="P8" s="99"/>
-      <c r="Q8" s="106"/>
-      <c r="R8" s="106"/>
-      <c r="S8" s="106"/>
-      <c r="T8" s="106"/>
-      <c r="U8" s="106"/>
-      <c r="V8" s="99"/>
-      <c r="W8" s="131"/>
+      <c r="O8" s="81"/>
+      <c r="P8" s="77"/>
+      <c r="Q8" s="81"/>
+      <c r="R8" s="81"/>
+      <c r="S8" s="81"/>
+      <c r="T8" s="81"/>
+      <c r="U8" s="81"/>
+      <c r="V8" s="77"/>
+      <c r="W8" s="97"/>
     </row>
     <row r="9" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B9" s="129">
+      <c r="B9" s="95">
         <v>6</v>
       </c>
-      <c r="C9" s="130"/>
-      <c r="D9" s="115">
+      <c r="C9" s="96"/>
+      <c r="D9" s="90">
         <v>42802</v>
       </c>
-      <c r="E9" s="106" t="s">
+      <c r="E9" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="106">
+      <c r="F9" s="81">
         <v>-0.1</v>
       </c>
-      <c r="G9" s="106" t="s">
+      <c r="G9" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="H9" s="106">
+      <c r="H9" s="81">
         <v>180</v>
       </c>
-      <c r="I9" s="106">
+      <c r="I9" s="81">
         <v>12</v>
       </c>
-      <c r="J9" s="106">
+      <c r="J9" s="81">
         <v>36</v>
       </c>
-      <c r="K9" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="L9" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="M9" s="99" t="s">
-        <v>34</v>
-      </c>
-      <c r="N9" s="110">
+      <c r="K9" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="L9" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="M9" s="77" t="s">
+        <v>34</v>
+      </c>
+      <c r="N9" s="85">
         <v>2</v>
       </c>
-      <c r="O9" s="106"/>
-      <c r="P9" s="99"/>
-      <c r="Q9" s="106"/>
-      <c r="R9" s="117">
+      <c r="O9" s="81"/>
+      <c r="P9" s="77"/>
+      <c r="Q9" s="81"/>
+      <c r="R9" s="92">
         <v>42985</v>
       </c>
-      <c r="S9" s="106"/>
-      <c r="T9" s="106"/>
-      <c r="U9" s="106"/>
-      <c r="V9" s="99"/>
-      <c r="W9" s="131"/>
+      <c r="S9" s="81"/>
+      <c r="T9" s="81"/>
+      <c r="U9" s="81"/>
+      <c r="V9" s="77"/>
+      <c r="W9" s="97"/>
     </row>
     <row r="10" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B10" s="129">
+      <c r="B10" s="95">
         <v>7</v>
       </c>
-      <c r="C10" s="130"/>
-      <c r="D10" s="115">
+      <c r="C10" s="96"/>
+      <c r="D10" s="90">
         <v>42803</v>
       </c>
-      <c r="E10" s="106" t="s">
+      <c r="E10" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="F10" s="106">
+      <c r="F10" s="81">
         <v>-0.1</v>
       </c>
-      <c r="G10" s="106" t="s">
+      <c r="G10" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="106">
+      <c r="H10" s="81">
         <v>180</v>
       </c>
-      <c r="I10" s="106">
+      <c r="I10" s="81">
         <v>12</v>
       </c>
-      <c r="J10" s="106">
+      <c r="J10" s="81">
         <v>45</v>
       </c>
-      <c r="K10" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="L10" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="M10" s="99" t="s">
-        <v>34</v>
-      </c>
-      <c r="N10" s="110" t="s">
+      <c r="K10" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="L10" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="M10" s="77" t="s">
+        <v>34</v>
+      </c>
+      <c r="N10" s="85" t="s">
         <v>57</v>
       </c>
-      <c r="O10" s="106"/>
-      <c r="P10" s="99"/>
-      <c r="Q10" s="117">
+      <c r="O10" s="81"/>
+      <c r="P10" s="77"/>
+      <c r="Q10" s="92">
         <v>42808</v>
       </c>
-      <c r="R10" s="117">
+      <c r="R10" s="92">
         <v>42985</v>
       </c>
-      <c r="S10" s="106"/>
-      <c r="T10" s="106"/>
-      <c r="U10" s="106"/>
-      <c r="V10" s="99"/>
-      <c r="W10" s="131"/>
+      <c r="S10" s="81"/>
+      <c r="T10" s="81"/>
+      <c r="U10" s="81"/>
+      <c r="V10" s="77"/>
+      <c r="W10" s="97"/>
     </row>
     <row r="11" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B11" s="129">
+      <c r="B11" s="95">
         <v>8</v>
       </c>
-      <c r="C11" s="130"/>
-      <c r="D11" s="115">
+      <c r="C11" s="96"/>
+      <c r="D11" s="90">
         <v>42899</v>
       </c>
-      <c r="E11" s="106" t="s">
+      <c r="E11" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="106">
+      <c r="F11" s="81">
         <v>-0.1</v>
       </c>
-      <c r="G11" s="106" t="s">
+      <c r="G11" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="H11" s="106">
+      <c r="H11" s="81">
         <v>180</v>
       </c>
-      <c r="I11" s="106">
+      <c r="I11" s="81">
         <v>12</v>
       </c>
-      <c r="J11" s="106" t="s">
+      <c r="J11" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="K11" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="L11" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="M11" s="99" t="s">
-        <v>34</v>
-      </c>
-      <c r="N11" s="110">
+      <c r="K11" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="L11" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="M11" s="77" t="s">
+        <v>34</v>
+      </c>
+      <c r="N11" s="85">
         <v>3</v>
       </c>
-      <c r="O11" s="106"/>
-      <c r="P11" s="99"/>
-      <c r="Q11" s="117">
+      <c r="O11" s="81"/>
+      <c r="P11" s="77"/>
+      <c r="Q11" s="92">
         <v>42961</v>
       </c>
-      <c r="R11" s="117">
+      <c r="R11" s="92">
         <v>42985</v>
       </c>
-      <c r="S11" s="106"/>
-      <c r="T11" s="106"/>
-      <c r="U11" s="106"/>
-      <c r="V11" s="99"/>
-      <c r="W11" s="131"/>
+      <c r="S11" s="81"/>
+      <c r="T11" s="81"/>
+      <c r="U11" s="81"/>
+      <c r="V11" s="77"/>
+      <c r="W11" s="97"/>
     </row>
     <row r="12" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B12" s="129">
+      <c r="B12" s="95">
         <v>9</v>
       </c>
-      <c r="C12" s="130"/>
-      <c r="D12" s="115">
+      <c r="C12" s="96"/>
+      <c r="D12" s="90">
         <v>42905</v>
       </c>
-      <c r="E12" s="106" t="s">
+      <c r="E12" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="F12" s="106">
+      <c r="F12" s="81">
         <v>-0.1</v>
       </c>
-      <c r="G12" s="106" t="s">
+      <c r="G12" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="H12" s="106">
+      <c r="H12" s="81">
         <v>240</v>
       </c>
-      <c r="I12" s="106">
+      <c r="I12" s="81">
         <v>12</v>
       </c>
-      <c r="J12" s="106" t="s">
+      <c r="J12" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="K12" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="L12" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="M12" s="99" t="s">
-        <v>34</v>
-      </c>
-      <c r="N12" s="110">
+      <c r="K12" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="L12" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="M12" s="77" t="s">
+        <v>34</v>
+      </c>
+      <c r="N12" s="85">
         <v>3</v>
       </c>
-      <c r="O12" s="106"/>
-      <c r="P12" s="99"/>
-      <c r="Q12" s="117">
+      <c r="O12" s="81"/>
+      <c r="P12" s="77"/>
+      <c r="Q12" s="92">
         <v>42961</v>
       </c>
-      <c r="R12" s="117">
+      <c r="R12" s="92">
         <v>42985</v>
       </c>
-      <c r="S12" s="106"/>
-      <c r="T12" s="106"/>
-      <c r="U12" s="106"/>
-      <c r="V12" s="99"/>
-      <c r="W12" s="131"/>
+      <c r="S12" s="81"/>
+      <c r="T12" s="81"/>
+      <c r="U12" s="81"/>
+      <c r="V12" s="77"/>
+      <c r="W12" s="97"/>
     </row>
     <row r="13" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B13" s="129">
+      <c r="B13" s="95">
         <v>10</v>
       </c>
-      <c r="C13" s="130"/>
-      <c r="D13" s="115">
+      <c r="C13" s="96"/>
+      <c r="D13" s="90">
         <v>42977</v>
       </c>
-      <c r="E13" s="106" t="s">
+      <c r="E13" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="106">
+      <c r="F13" s="81">
         <v>-0.1</v>
       </c>
-      <c r="G13" s="106" t="s">
+      <c r="G13" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="H13" s="106">
+      <c r="H13" s="81">
         <v>180</v>
       </c>
-      <c r="I13" s="106">
+      <c r="I13" s="81">
         <v>11</v>
       </c>
-      <c r="J13" s="106" t="s">
+      <c r="J13" s="81" t="s">
         <v>40</v>
       </c>
-      <c r="K13" s="106" t="s">
+      <c r="K13" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="L13" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="M13" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="N13" s="111">
+      <c r="L13" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="M13" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="N13" s="86">
         <v>4</v>
       </c>
-      <c r="O13" s="100">
+      <c r="O13" s="78">
         <f>Electrolytes!$M$4</f>
         <v>47.6</v>
       </c>
-      <c r="P13" s="101"/>
-      <c r="Q13" s="117">
+      <c r="P13" s="79"/>
+      <c r="Q13" s="92">
         <v>43014</v>
       </c>
-      <c r="R13" s="117">
+      <c r="R13" s="92">
         <v>42985</v>
       </c>
-      <c r="S13" s="106"/>
-      <c r="T13" s="106"/>
-      <c r="U13" s="106"/>
-      <c r="V13" s="99"/>
-      <c r="W13" s="131"/>
+      <c r="S13" s="81"/>
+      <c r="T13" s="81"/>
+      <c r="U13" s="81"/>
+      <c r="V13" s="77"/>
+      <c r="W13" s="97"/>
     </row>
     <row r="14" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B14" s="129">
+      <c r="B14" s="95">
         <v>11</v>
       </c>
-      <c r="C14" s="130"/>
-      <c r="D14" s="115">
+      <c r="C14" s="96"/>
+      <c r="D14" s="90">
         <v>42978</v>
       </c>
-      <c r="E14" s="106" t="s">
+      <c r="E14" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="F14" s="106">
+      <c r="F14" s="81">
         <v>-0.1</v>
       </c>
-      <c r="G14" s="106" t="s">
+      <c r="G14" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="H14" s="106">
+      <c r="H14" s="81">
         <v>180</v>
       </c>
-      <c r="I14" s="106">
+      <c r="I14" s="81">
         <v>11</v>
       </c>
-      <c r="J14" s="106" t="s">
+      <c r="J14" s="81" t="s">
         <v>41</v>
       </c>
-      <c r="K14" s="106" t="s">
+      <c r="K14" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="L14" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="M14" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="N14" s="112">
+      <c r="L14" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="M14" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="N14" s="87">
         <v>4</v>
       </c>
-      <c r="O14" s="106"/>
-      <c r="P14" s="99"/>
-      <c r="Q14" s="117">
+      <c r="O14" s="81"/>
+      <c r="P14" s="77"/>
+      <c r="Q14" s="92">
         <v>43014</v>
       </c>
-      <c r="R14" s="117">
+      <c r="R14" s="92">
         <v>42985</v>
       </c>
-      <c r="S14" s="106"/>
-      <c r="T14" s="106"/>
-      <c r="U14" s="106"/>
-      <c r="V14" s="99"/>
-      <c r="W14" s="131"/>
+      <c r="S14" s="81"/>
+      <c r="T14" s="81"/>
+      <c r="U14" s="81"/>
+      <c r="V14" s="77"/>
+      <c r="W14" s="97"/>
     </row>
     <row r="15" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B15" s="129">
+      <c r="B15" s="95">
         <v>12</v>
       </c>
-      <c r="C15" s="130"/>
-      <c r="D15" s="115">
+      <c r="C15" s="96"/>
+      <c r="D15" s="90">
         <v>42979</v>
       </c>
-      <c r="E15" s="106" t="s">
+      <c r="E15" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="F15" s="106">
+      <c r="F15" s="81">
         <v>-0.1</v>
       </c>
-      <c r="G15" s="106" t="s">
+      <c r="G15" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="H15" s="106">
+      <c r="H15" s="81">
         <v>180</v>
       </c>
-      <c r="I15" s="106">
+      <c r="I15" s="81">
         <v>11</v>
       </c>
-      <c r="J15" s="106">
+      <c r="J15" s="81">
         <v>30</v>
       </c>
-      <c r="K15" s="106" t="s">
+      <c r="K15" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="L15" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="M15" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="N15" s="112">
+      <c r="L15" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="M15" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="N15" s="87">
         <v>4</v>
       </c>
-      <c r="O15" s="106"/>
-      <c r="P15" s="99"/>
-      <c r="Q15" s="117">
+      <c r="O15" s="81"/>
+      <c r="P15" s="77"/>
+      <c r="Q15" s="92">
         <v>43014</v>
       </c>
-      <c r="R15" s="117">
+      <c r="R15" s="92">
         <v>42985</v>
       </c>
-      <c r="S15" s="106"/>
-      <c r="T15" s="106"/>
-      <c r="U15" s="106"/>
-      <c r="V15" s="99"/>
-      <c r="W15" s="131"/>
+      <c r="S15" s="81"/>
+      <c r="T15" s="81"/>
+      <c r="U15" s="81"/>
+      <c r="V15" s="77"/>
+      <c r="W15" s="97"/>
     </row>
     <row r="16" spans="2:23" ht="32" x14ac:dyDescent="0.2">
-      <c r="B16" s="129">
+      <c r="B16" s="95">
         <v>13</v>
       </c>
-      <c r="C16" s="130"/>
-      <c r="D16" s="115">
+      <c r="C16" s="96"/>
+      <c r="D16" s="90">
         <v>42983</v>
       </c>
-      <c r="E16" s="106" t="s">
+      <c r="E16" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="F16" s="106">
+      <c r="F16" s="81">
         <v>-0.1</v>
       </c>
-      <c r="G16" s="106" t="s">
+      <c r="G16" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="H16" s="106">
+      <c r="H16" s="81">
         <v>180</v>
       </c>
-      <c r="I16" s="106">
+      <c r="I16" s="81">
         <v>11</v>
       </c>
-      <c r="J16" s="106">
+      <c r="J16" s="81">
         <v>30</v>
       </c>
-      <c r="K16" s="106" t="s">
+      <c r="K16" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="L16" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="M16" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="N16" s="112">
+      <c r="L16" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="M16" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="N16" s="87">
         <v>4</v>
       </c>
-      <c r="O16" s="106"/>
-      <c r="P16" s="99"/>
-      <c r="Q16" s="117">
+      <c r="O16" s="81"/>
+      <c r="P16" s="77"/>
+      <c r="Q16" s="92">
         <v>43014</v>
       </c>
-      <c r="R16" s="117">
+      <c r="R16" s="92">
         <v>42985</v>
       </c>
-      <c r="S16" s="106"/>
-      <c r="T16" s="106"/>
-      <c r="U16" s="106"/>
-      <c r="V16" s="99"/>
-      <c r="W16" s="132" t="s">
+      <c r="S16" s="81"/>
+      <c r="T16" s="81"/>
+      <c r="U16" s="81"/>
+      <c r="V16" s="77"/>
+      <c r="W16" s="98" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="17" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B17" s="129">
+      <c r="B17" s="95">
         <v>14</v>
       </c>
-      <c r="C17" s="130"/>
-      <c r="D17" s="115">
+      <c r="C17" s="96"/>
+      <c r="D17" s="90">
         <v>42984</v>
       </c>
-      <c r="E17" s="106" t="s">
+      <c r="E17" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="106">
+      <c r="F17" s="81">
         <v>-0.1</v>
       </c>
-      <c r="G17" s="106" t="s">
+      <c r="G17" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="H17" s="106">
+      <c r="H17" s="81">
         <v>240</v>
       </c>
-      <c r="I17" s="106">
+      <c r="I17" s="81">
         <v>11</v>
       </c>
-      <c r="J17" s="106" t="s">
+      <c r="J17" s="81" t="s">
         <v>55</v>
       </c>
-      <c r="K17" s="106" t="s">
+      <c r="K17" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="L17" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="M17" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="N17" s="113">
+      <c r="L17" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="M17" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="N17" s="88">
         <v>4</v>
       </c>
-      <c r="O17" s="102">
+      <c r="O17" s="80">
         <v>40</v>
       </c>
-      <c r="P17" s="99"/>
-      <c r="Q17" s="106"/>
-      <c r="R17" s="117">
+      <c r="P17" s="77"/>
+      <c r="Q17" s="81"/>
+      <c r="R17" s="92">
         <v>42990</v>
       </c>
-      <c r="S17" s="106"/>
-      <c r="T17" s="106"/>
-      <c r="U17" s="106"/>
-      <c r="V17" s="99"/>
-      <c r="W17" s="131"/>
+      <c r="S17" s="81"/>
+      <c r="T17" s="81"/>
+      <c r="U17" s="81"/>
+      <c r="V17" s="77"/>
+      <c r="W17" s="97"/>
     </row>
     <row r="18" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B18" s="133">
+      <c r="B18" s="99">
         <v>15</v>
       </c>
-      <c r="C18" s="130"/>
-      <c r="D18" s="115">
+      <c r="C18" s="96"/>
+      <c r="D18" s="90">
         <v>42985</v>
       </c>
-      <c r="E18" s="106" t="s">
+      <c r="E18" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="F18" s="106">
+      <c r="F18" s="81">
         <v>-0.1</v>
       </c>
-      <c r="G18" s="106" t="s">
+      <c r="G18" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="H18" s="106">
+      <c r="H18" s="81">
         <v>120</v>
       </c>
-      <c r="I18" s="106">
+      <c r="I18" s="81">
         <v>12</v>
       </c>
-      <c r="J18" s="106">
+      <c r="J18" s="81">
         <v>30</v>
       </c>
-      <c r="K18" s="106" t="s">
+      <c r="K18" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="L18" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="M18" s="99" t="s">
-        <v>34</v>
-      </c>
-      <c r="N18" s="112">
+      <c r="L18" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="M18" s="77" t="s">
+        <v>34</v>
+      </c>
+      <c r="N18" s="87">
         <v>5</v>
       </c>
-      <c r="O18" s="100">
+      <c r="O18" s="78">
         <f>Electrolytes!$M$5</f>
         <v>71</v>
       </c>
-      <c r="P18" s="101"/>
-      <c r="Q18" s="106"/>
-      <c r="R18" s="117">
+      <c r="P18" s="79"/>
+      <c r="Q18" s="81"/>
+      <c r="R18" s="92">
         <v>42990</v>
       </c>
-      <c r="S18" s="106"/>
-      <c r="T18" s="106"/>
-      <c r="U18" s="106"/>
-      <c r="V18" s="99"/>
-      <c r="W18" s="131"/>
+      <c r="S18" s="81"/>
+      <c r="T18" s="81"/>
+      <c r="U18" s="81"/>
+      <c r="V18" s="77"/>
+      <c r="W18" s="97"/>
     </row>
     <row r="19" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B19" s="133">
+      <c r="B19" s="99">
         <v>16</v>
       </c>
-      <c r="C19" s="130"/>
-      <c r="D19" s="115">
+      <c r="C19" s="96"/>
+      <c r="D19" s="90">
         <v>42986</v>
       </c>
-      <c r="E19" s="106" t="s">
+      <c r="E19" s="81" t="s">
         <v>62</v>
       </c>
-      <c r="F19" s="106">
+      <c r="F19" s="81">
         <v>-0.1</v>
       </c>
-      <c r="G19" s="106" t="s">
+      <c r="G19" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="H19" s="106">
+      <c r="H19" s="81">
         <v>180</v>
       </c>
-      <c r="I19" s="106">
+      <c r="I19" s="81">
         <v>12</v>
       </c>
-      <c r="J19" s="106" t="s">
+      <c r="J19" s="81" t="s">
         <v>63</v>
       </c>
-      <c r="K19" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="L19" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="M19" s="99" t="s">
-        <v>34</v>
-      </c>
-      <c r="N19" s="112">
+      <c r="K19" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="L19" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="M19" s="77" t="s">
+        <v>34</v>
+      </c>
+      <c r="N19" s="87">
         <v>5</v>
       </c>
-      <c r="O19" s="106"/>
-      <c r="P19" s="99"/>
-      <c r="Q19" s="106"/>
-      <c r="R19" s="117">
+      <c r="O19" s="81"/>
+      <c r="P19" s="77"/>
+      <c r="Q19" s="81"/>
+      <c r="R19" s="92">
         <v>42990</v>
       </c>
-      <c r="S19" s="106"/>
-      <c r="T19" s="106"/>
-      <c r="U19" s="106"/>
-      <c r="V19" s="99"/>
-      <c r="W19" s="131" t="s">
+      <c r="S19" s="81"/>
+      <c r="T19" s="81"/>
+      <c r="U19" s="81"/>
+      <c r="V19" s="77"/>
+      <c r="W19" s="97" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="20" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="133">
+      <c r="B20" s="99">
         <v>17</v>
       </c>
-      <c r="C20" s="130"/>
-      <c r="D20" s="116">
+      <c r="C20" s="96"/>
+      <c r="D20" s="91">
         <v>42990</v>
       </c>
-      <c r="E20" s="106" t="s">
+      <c r="E20" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="F20" s="106">
+      <c r="F20" s="81">
         <v>-0.1</v>
       </c>
-      <c r="G20" s="106" t="s">
+      <c r="G20" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="H20" s="106">
+      <c r="H20" s="81">
         <v>240</v>
       </c>
-      <c r="I20" s="106">
+      <c r="I20" s="81">
         <v>12</v>
       </c>
-      <c r="J20" s="106" t="s">
+      <c r="J20" s="81" t="s">
         <v>63</v>
       </c>
-      <c r="K20" s="106" t="s">
+      <c r="K20" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="L20" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="M20" s="108" t="s">
-        <v>34</v>
-      </c>
-      <c r="N20" s="112">
+      <c r="L20" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="M20" s="83" t="s">
+        <v>34</v>
+      </c>
+      <c r="N20" s="87">
         <v>5</v>
       </c>
-      <c r="O20" s="106"/>
-      <c r="P20" s="108"/>
-      <c r="Q20" s="106"/>
-      <c r="R20" s="117">
+      <c r="O20" s="81"/>
+      <c r="P20" s="83"/>
+      <c r="Q20" s="81"/>
+      <c r="R20" s="92">
         <v>42997</v>
       </c>
-      <c r="S20" s="106"/>
-      <c r="T20" s="106"/>
-      <c r="U20" s="106"/>
-      <c r="V20" s="108"/>
-      <c r="W20" s="131"/>
+      <c r="S20" s="81"/>
+      <c r="T20" s="81"/>
+      <c r="U20" s="81"/>
+      <c r="V20" s="83"/>
+      <c r="W20" s="97"/>
     </row>
     <row r="21" spans="2:23" ht="22" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="103" t="s">
+      <c r="B21" s="115" t="s">
         <v>75</v>
       </c>
-      <c r="C21" s="104"/>
-      <c r="D21" s="104"/>
-      <c r="E21" s="104"/>
-      <c r="F21" s="104"/>
-      <c r="G21" s="104"/>
-      <c r="H21" s="104"/>
-      <c r="I21" s="104"/>
-      <c r="J21" s="104"/>
-      <c r="K21" s="104"/>
-      <c r="L21" s="104"/>
-      <c r="M21" s="104"/>
-      <c r="N21" s="104"/>
-      <c r="O21" s="104"/>
-      <c r="P21" s="104"/>
-      <c r="Q21" s="104"/>
-      <c r="R21" s="104"/>
-      <c r="S21" s="104"/>
-      <c r="T21" s="104"/>
-      <c r="U21" s="104"/>
-      <c r="V21" s="104"/>
-      <c r="W21" s="105"/>
+      <c r="C21" s="116"/>
+      <c r="D21" s="116"/>
+      <c r="E21" s="116"/>
+      <c r="F21" s="116"/>
+      <c r="G21" s="116"/>
+      <c r="H21" s="116"/>
+      <c r="I21" s="116"/>
+      <c r="J21" s="116"/>
+      <c r="K21" s="116"/>
+      <c r="L21" s="116"/>
+      <c r="M21" s="116"/>
+      <c r="N21" s="116"/>
+      <c r="O21" s="116"/>
+      <c r="P21" s="116"/>
+      <c r="Q21" s="116"/>
+      <c r="R21" s="116"/>
+      <c r="S21" s="116"/>
+      <c r="T21" s="116"/>
+      <c r="U21" s="116"/>
+      <c r="V21" s="116"/>
+      <c r="W21" s="117"/>
     </row>
     <row r="22" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B22" s="133">
+      <c r="B22" s="99">
         <v>18</v>
       </c>
-      <c r="C22" s="130"/>
-      <c r="D22" s="115">
+      <c r="C22" s="96"/>
+      <c r="D22" s="90">
         <v>42996</v>
       </c>
-      <c r="E22" s="106" t="s">
+      <c r="E22" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="F22" s="106">
+      <c r="F22" s="81">
         <v>-0.1</v>
       </c>
-      <c r="G22" s="106" t="s">
+      <c r="G22" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="H22" s="106">
+      <c r="H22" s="81">
         <v>180</v>
       </c>
-      <c r="I22" s="106">
+      <c r="I22" s="81">
         <v>12</v>
       </c>
-      <c r="J22" s="106" t="s">
+      <c r="J22" s="81" t="s">
         <v>63</v>
       </c>
-      <c r="K22" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="L22" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="M22" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="N22" s="112">
+      <c r="K22" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="L22" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="M22" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="N22" s="87">
         <v>6</v>
       </c>
-      <c r="O22" s="106"/>
-      <c r="P22" s="99"/>
-      <c r="Q22" s="106"/>
-      <c r="R22" s="117">
+      <c r="O22" s="81"/>
+      <c r="P22" s="77"/>
+      <c r="Q22" s="81"/>
+      <c r="R22" s="92">
         <v>42997</v>
       </c>
-      <c r="S22" s="106"/>
-      <c r="T22" s="106"/>
-      <c r="U22" s="106"/>
-      <c r="V22" s="99"/>
-      <c r="W22" s="131"/>
+      <c r="S22" s="81"/>
+      <c r="T22" s="81"/>
+      <c r="U22" s="81"/>
+      <c r="V22" s="77"/>
+      <c r="W22" s="97"/>
     </row>
     <row r="23" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B23" s="133">
+      <c r="B23" s="99">
         <v>19</v>
       </c>
-      <c r="C23" s="130"/>
-      <c r="D23" s="115">
+      <c r="C23" s="96"/>
+      <c r="D23" s="90">
         <v>42996</v>
       </c>
-      <c r="E23" s="106" t="s">
+      <c r="E23" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="F23" s="106">
+      <c r="F23" s="81">
         <v>-0.1</v>
       </c>
-      <c r="G23" s="106" t="s">
+      <c r="G23" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="H23" s="106">
+      <c r="H23" s="81">
         <v>180</v>
       </c>
-      <c r="I23" s="106">
+      <c r="I23" s="81">
         <v>12</v>
       </c>
-      <c r="J23" s="106" t="s">
+      <c r="J23" s="81" t="s">
         <v>80</v>
       </c>
-      <c r="K23" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="L23" s="106" t="s">
+      <c r="K23" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="L23" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="M23" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="N23" s="112">
+      <c r="M23" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="N23" s="87">
         <v>6</v>
       </c>
-      <c r="O23" s="106"/>
-      <c r="P23" s="99"/>
-      <c r="Q23" s="106"/>
-      <c r="R23" s="117">
+      <c r="O23" s="81"/>
+      <c r="P23" s="77"/>
+      <c r="Q23" s="81"/>
+      <c r="R23" s="92">
         <v>42997</v>
       </c>
-      <c r="S23" s="106"/>
-      <c r="T23" s="106"/>
-      <c r="U23" s="106"/>
-      <c r="V23" s="99"/>
-      <c r="W23" s="131"/>
+      <c r="S23" s="81"/>
+      <c r="T23" s="81"/>
+      <c r="U23" s="81"/>
+      <c r="V23" s="77"/>
+      <c r="W23" s="97"/>
     </row>
     <row r="24" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B24" s="133">
+      <c r="B24" s="99">
         <v>20</v>
       </c>
-      <c r="C24" s="130"/>
-      <c r="D24" s="115">
+      <c r="C24" s="96"/>
+      <c r="D24" s="90">
         <v>42997</v>
       </c>
-      <c r="E24" s="106" t="s">
+      <c r="E24" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="F24" s="106">
+      <c r="F24" s="81">
         <v>-0.1</v>
       </c>
-      <c r="G24" s="106" t="s">
+      <c r="G24" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="H24" s="106">
+      <c r="H24" s="81">
         <v>180</v>
       </c>
-      <c r="I24" s="106">
+      <c r="I24" s="81">
         <v>12</v>
       </c>
-      <c r="J24" s="106" t="s">
+      <c r="J24" s="81" t="s">
         <v>80</v>
       </c>
-      <c r="K24" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="L24" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="M24" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="N24" s="112">
+      <c r="K24" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="L24" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="M24" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="N24" s="87">
         <v>6</v>
       </c>
-      <c r="O24" s="106"/>
-      <c r="P24" s="99"/>
-      <c r="Q24" s="106"/>
-      <c r="R24" s="106"/>
-      <c r="S24" s="106"/>
-      <c r="T24" s="106"/>
-      <c r="U24" s="106"/>
-      <c r="V24" s="99"/>
-      <c r="W24" s="131"/>
+      <c r="O24" s="81"/>
+      <c r="P24" s="77"/>
+      <c r="Q24" s="81"/>
+      <c r="R24" s="81"/>
+      <c r="S24" s="81"/>
+      <c r="T24" s="81"/>
+      <c r="U24" s="81"/>
+      <c r="V24" s="77"/>
+      <c r="W24" s="97"/>
     </row>
     <row r="25" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B25" s="133">
+      <c r="B25" s="99">
         <v>21</v>
       </c>
-      <c r="C25" s="130"/>
-      <c r="D25" s="115">
+      <c r="C25" s="96"/>
+      <c r="D25" s="90">
         <v>42997</v>
       </c>
-      <c r="E25" s="106" t="s">
+      <c r="E25" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="F25" s="106">
+      <c r="F25" s="81">
         <v>-0.1</v>
       </c>
-      <c r="G25" s="106" t="s">
+      <c r="G25" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="H25" s="106">
+      <c r="H25" s="81">
         <v>180</v>
       </c>
-      <c r="I25" s="106">
+      <c r="I25" s="81">
         <v>12</v>
       </c>
-      <c r="J25" s="106">
+      <c r="J25" s="81">
         <v>40</v>
       </c>
-      <c r="K25" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="L25" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="M25" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="N25" s="112">
+      <c r="K25" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="L25" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="M25" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="N25" s="87">
         <v>6</v>
       </c>
-      <c r="O25" s="106"/>
-      <c r="P25" s="99"/>
-      <c r="Q25" s="106"/>
-      <c r="R25" s="106"/>
-      <c r="S25" s="106"/>
-      <c r="T25" s="106"/>
-      <c r="U25" s="106"/>
-      <c r="V25" s="99"/>
-      <c r="W25" s="131"/>
+      <c r="O25" s="81"/>
+      <c r="P25" s="77"/>
+      <c r="Q25" s="81"/>
+      <c r="R25" s="81"/>
+      <c r="S25" s="81"/>
+      <c r="T25" s="81"/>
+      <c r="U25" s="81"/>
+      <c r="V25" s="77"/>
+      <c r="W25" s="97"/>
     </row>
     <row r="26" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B26" s="133">
+      <c r="B26" s="99">
         <v>22</v>
       </c>
-      <c r="C26" s="130"/>
-      <c r="D26" s="115">
+      <c r="C26" s="96"/>
+      <c r="D26" s="90">
         <v>42997</v>
       </c>
-      <c r="E26" s="106" t="s">
+      <c r="E26" s="81" t="s">
         <v>29</v>
       </c>
-      <c r="F26" s="106">
+      <c r="F26" s="81">
         <v>-0.1</v>
       </c>
-      <c r="G26" s="106" t="s">
+      <c r="G26" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="H26" s="106">
+      <c r="H26" s="81">
         <v>300</v>
       </c>
-      <c r="I26" s="106">
+      <c r="I26" s="81">
         <v>12</v>
       </c>
-      <c r="J26" s="106">
+      <c r="J26" s="81">
         <v>40</v>
       </c>
-      <c r="K26" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="L26" s="106" t="s">
+      <c r="K26" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="L26" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="M26" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="N26" s="113">
+      <c r="M26" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="N26" s="88">
         <v>6</v>
       </c>
-      <c r="O26" s="106"/>
-      <c r="P26" s="99"/>
-      <c r="Q26" s="106"/>
-      <c r="R26" s="106"/>
-      <c r="S26" s="106"/>
-      <c r="T26" s="106"/>
-      <c r="U26" s="106"/>
-      <c r="V26" s="99"/>
-      <c r="W26" s="131"/>
+      <c r="O26" s="81"/>
+      <c r="P26" s="77"/>
+      <c r="Q26" s="81"/>
+      <c r="R26" s="81"/>
+      <c r="S26" s="81"/>
+      <c r="T26" s="81"/>
+      <c r="U26" s="81"/>
+      <c r="V26" s="77"/>
+      <c r="W26" s="97"/>
     </row>
     <row r="27" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B27" s="133">
+      <c r="B27" s="99">
         <v>23</v>
       </c>
-      <c r="C27" s="134"/>
-      <c r="D27" s="115">
+      <c r="C27" s="100"/>
+      <c r="D27" s="90">
         <v>43006</v>
       </c>
-      <c r="E27" s="106" t="s">
+      <c r="E27" s="81" t="s">
         <v>81</v>
       </c>
-      <c r="F27" s="106">
+      <c r="F27" s="81">
         <v>-0.1</v>
       </c>
-      <c r="G27" s="106" t="s">
+      <c r="G27" s="81" t="s">
         <v>37</v>
       </c>
-      <c r="H27" s="106">
+      <c r="H27" s="81">
         <v>180</v>
       </c>
-      <c r="I27" s="106">
+      <c r="I27" s="81">
         <v>12</v>
       </c>
-      <c r="J27" s="106" t="s">
+      <c r="J27" s="81" t="s">
         <v>55</v>
       </c>
-      <c r="K27" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="L27" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="M27" s="106" t="s">
-        <v>34</v>
-      </c>
-      <c r="N27" s="112">
+      <c r="K27" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="L27" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="M27" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="N27" s="87">
         <v>7</v>
       </c>
-      <c r="O27" s="140">
+      <c r="O27" s="106">
         <f>Electrolytes!M8</f>
         <v>50</v>
       </c>
-      <c r="P27" s="101"/>
-      <c r="Q27" s="106"/>
-      <c r="R27" s="106"/>
-      <c r="S27" s="106"/>
-      <c r="T27" s="106"/>
-      <c r="U27" s="106"/>
-      <c r="V27" s="99"/>
-      <c r="W27" s="131"/>
+      <c r="P27" s="79"/>
+      <c r="Q27" s="81"/>
+      <c r="R27" s="81"/>
+      <c r="S27" s="81"/>
+      <c r="T27" s="81"/>
+      <c r="U27" s="81"/>
+      <c r="V27" s="77"/>
+      <c r="W27" s="97"/>
     </row>
     <row r="28" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="B28" s="133"/>
-      <c r="C28" s="106"/>
-      <c r="D28" s="115"/>
-      <c r="E28" s="106"/>
-      <c r="F28" s="106"/>
-      <c r="G28" s="106"/>
-      <c r="H28" s="106"/>
-      <c r="I28" s="106"/>
-      <c r="J28" s="106"/>
-      <c r="K28" s="106"/>
-      <c r="L28" s="106"/>
-      <c r="N28" s="110"/>
-      <c r="O28" s="106"/>
-      <c r="Q28" s="94"/>
-      <c r="R28" s="106"/>
-      <c r="S28" s="106"/>
-      <c r="T28" s="106"/>
-      <c r="U28" s="106"/>
-      <c r="V28" s="99"/>
-      <c r="W28" s="131"/>
+      <c r="B28" s="99">
+        <v>24</v>
+      </c>
+      <c r="C28" s="141"/>
+      <c r="D28" s="90">
+        <v>43006</v>
+      </c>
+      <c r="E28" s="81" t="s">
+        <v>81</v>
+      </c>
+      <c r="F28" s="81">
+        <v>-0.1</v>
+      </c>
+      <c r="G28" s="81" t="s">
+        <v>37</v>
+      </c>
+      <c r="H28" s="81">
+        <v>240</v>
+      </c>
+      <c r="I28" s="81">
+        <v>12</v>
+      </c>
+      <c r="J28" s="81" t="s">
+        <v>55</v>
+      </c>
+      <c r="K28" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="L28" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="M28" s="81" t="s">
+        <v>34</v>
+      </c>
+      <c r="N28" s="87">
+        <v>7</v>
+      </c>
+      <c r="O28" s="81"/>
+      <c r="Q28" s="72"/>
+      <c r="R28" s="81"/>
+      <c r="S28" s="81"/>
+      <c r="T28" s="81"/>
+      <c r="U28" s="81"/>
+      <c r="V28" s="77"/>
+      <c r="W28" s="97"/>
     </row>
     <row r="29" spans="2:23" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="135"/>
-      <c r="C29" s="136"/>
-      <c r="D29" s="116"/>
-      <c r="E29" s="136"/>
-      <c r="F29" s="136"/>
-      <c r="G29" s="136"/>
-      <c r="H29" s="136"/>
-      <c r="I29" s="136"/>
-      <c r="J29" s="136"/>
-      <c r="K29" s="136"/>
-      <c r="L29" s="136"/>
-      <c r="M29" s="136"/>
-      <c r="N29" s="137"/>
-      <c r="O29" s="136"/>
-      <c r="P29" s="136"/>
-      <c r="Q29" s="138"/>
-      <c r="R29" s="136"/>
-      <c r="S29" s="136"/>
-      <c r="T29" s="136"/>
-      <c r="U29" s="136"/>
-      <c r="V29" s="108"/>
-      <c r="W29" s="139"/>
+      <c r="B29" s="101"/>
+      <c r="C29" s="102"/>
+      <c r="D29" s="91"/>
+      <c r="E29" s="102"/>
+      <c r="F29" s="102"/>
+      <c r="G29" s="102"/>
+      <c r="H29" s="102"/>
+      <c r="I29" s="102"/>
+      <c r="J29" s="102"/>
+      <c r="K29" s="102"/>
+      <c r="L29" s="102"/>
+      <c r="M29" s="102"/>
+      <c r="N29" s="103"/>
+      <c r="O29" s="102"/>
+      <c r="P29" s="102"/>
+      <c r="Q29" s="104"/>
+      <c r="R29" s="102"/>
+      <c r="S29" s="102"/>
+      <c r="T29" s="102"/>
+      <c r="U29" s="102"/>
+      <c r="V29" s="83"/>
+      <c r="W29" s="105"/>
     </row>
     <row r="30" spans="2:23" x14ac:dyDescent="0.2">
-      <c r="D30" s="117"/>
+      <c r="D30" s="92"/>
     </row>
     <row r="33" spans="8:8" x14ac:dyDescent="0.2">
-      <c r="H33" s="93" t="s">
+      <c r="H33" s="71" t="s">
         <v>78</v>
       </c>
     </row>
@@ -3136,6 +3170,7 @@
     <hyperlink ref="N17" location="Electrolytes!B4" display="Electrolytes!B4"/>
     <hyperlink ref="N19:N20" location="Electrolytes!B5" display="Electrolytes!B5"/>
     <hyperlink ref="N13:N16" location="Electrolytes!A3" display="Electrolytes!A3"/>
+    <hyperlink ref="N28" location="Electrolytes!B8" display="Electrolytes!B8"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3146,7 +3181,7 @@
   <dimension ref="B1:N12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3162,81 +3197,81 @@
     <col min="9" max="9" width="10.33203125" style="15" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.83203125" style="15" customWidth="1"/>
     <col min="11" max="11" width="13" style="15" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" style="57" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.6640625" style="42" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.83203125" style="16" customWidth="1"/>
     <col min="14" max="16384" width="10.83203125" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:14" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B2" s="72" t="s">
+      <c r="B2" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="C2" s="73" t="s">
+      <c r="C2" s="124" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="73" t="s">
+      <c r="D2" s="126"/>
+      <c r="E2" s="126"/>
+      <c r="F2" s="125"/>
+      <c r="G2" s="124" t="s">
         <v>51</v>
       </c>
-      <c r="H2" s="75"/>
-      <c r="I2" s="73" t="s">
+      <c r="H2" s="125"/>
+      <c r="I2" s="124" t="s">
         <v>50</v>
       </c>
-      <c r="J2" s="74"/>
-      <c r="K2" s="74"/>
-      <c r="L2" s="74"/>
-      <c r="M2" s="75"/>
-      <c r="N2" s="76" t="s">
+      <c r="J2" s="126"/>
+      <c r="K2" s="126"/>
+      <c r="L2" s="126"/>
+      <c r="M2" s="125"/>
+      <c r="N2" s="130" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="3" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B3" s="77" t="s">
+      <c r="B3" s="56" t="s">
         <v>45</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="D3" s="56" t="s">
+      <c r="D3" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="56" t="s">
+      <c r="E3" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="56" t="s">
+      <c r="F3" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="G3" s="56" t="s">
+      <c r="G3" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="H3" s="56" t="s">
+      <c r="H3" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="I3" s="56" t="s">
+      <c r="I3" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="J3" s="56" t="s">
+      <c r="J3" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="K3" s="56" t="s">
+      <c r="K3" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="L3" s="56" t="s">
+      <c r="L3" s="41" t="s">
         <v>60</v>
       </c>
-      <c r="M3" s="56" t="s">
+      <c r="M3" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="N3" s="78"/>
+      <c r="N3" s="131"/>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B4" s="79">
+      <c r="B4" s="57">
         <v>4</v>
       </c>
-      <c r="C4" s="60">
+      <c r="C4" s="43">
         <v>0.2</v>
       </c>
       <c r="D4" s="18">
@@ -3257,26 +3292,26 @@
       <c r="I4" s="39">
         <v>11</v>
       </c>
-      <c r="J4" s="63">
-        <f>C4*($F4/$M4)</f>
+      <c r="J4" s="46">
+        <f t="shared" ref="J4:L5" si="0">C4*($F4/$M4)</f>
         <v>8.4033613445378158E-2</v>
       </c>
-      <c r="K4" s="63">
-        <f>D4*($F4/$M4)</f>
+      <c r="K4" s="46">
+        <f t="shared" si="0"/>
         <v>1.2605042016806722</v>
       </c>
-      <c r="L4" s="63">
-        <f>E4*($F4/$M4)</f>
+      <c r="L4" s="46">
+        <f t="shared" si="0"/>
         <v>0.21008403361344538</v>
       </c>
-      <c r="M4" s="57">
+      <c r="M4" s="42">
         <f>F4+H4</f>
         <v>47.6</v>
       </c>
-      <c r="N4" s="80"/>
+      <c r="N4" s="58"/>
     </row>
     <row r="5" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="81">
+      <c r="B5" s="59">
         <v>5</v>
       </c>
       <c r="C5" s="38">
@@ -3300,103 +3335,103 @@
       <c r="I5" s="39">
         <v>12</v>
       </c>
-      <c r="J5" s="63">
-        <f>C5*($F5/$M5)</f>
+      <c r="J5" s="46">
+        <f t="shared" si="0"/>
         <v>5.6338028169014093E-2</v>
       </c>
-      <c r="K5" s="63">
-        <f>D5*($F5/$M5)</f>
+      <c r="K5" s="46">
+        <f t="shared" si="0"/>
         <v>0.84507042253521125</v>
       </c>
-      <c r="L5" s="63">
-        <f>E5*($F5/$M5)</f>
+      <c r="L5" s="46">
+        <f t="shared" si="0"/>
         <v>0.14084507042253522</v>
       </c>
-      <c r="M5" s="57">
+      <c r="M5" s="42">
         <f>F5+H5</f>
         <v>71</v>
       </c>
-      <c r="N5" s="82">
+      <c r="N5" s="60">
         <v>42985</v>
       </c>
     </row>
     <row r="6" spans="2:14" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="58" t="s">
+      <c r="B6" s="127" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="59"/>
-      <c r="K6" s="59"/>
-      <c r="L6" s="59"/>
-      <c r="M6" s="59"/>
-      <c r="N6" s="46"/>
+      <c r="C6" s="128"/>
+      <c r="D6" s="128"/>
+      <c r="E6" s="128"/>
+      <c r="F6" s="128"/>
+      <c r="G6" s="128"/>
+      <c r="H6" s="128"/>
+      <c r="I6" s="128"/>
+      <c r="J6" s="128"/>
+      <c r="K6" s="128"/>
+      <c r="L6" s="128"/>
+      <c r="M6" s="128"/>
+      <c r="N6" s="129"/>
     </row>
     <row r="7" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B7" s="81">
+      <c r="B7" s="59">
         <v>6</v>
       </c>
-      <c r="C7" s="65">
+      <c r="C7" s="48">
         <f>'Stock Solutions'!$M$4</f>
         <v>0.2001378359751895</v>
       </c>
-      <c r="D7" s="66">
+      <c r="D7" s="49">
         <f>'Stock Solutions'!$O$4</f>
         <v>2.9950044404973353</v>
       </c>
-      <c r="E7" s="66">
+      <c r="E7" s="49">
         <f>'Stock Solutions'!$N$4</f>
         <v>0.50004592949822024</v>
       </c>
-      <c r="F7" s="67">
+      <c r="F7" s="50">
         <v>10</v>
       </c>
-      <c r="G7" s="68">
+      <c r="G7" s="51">
         <v>2</v>
       </c>
-      <c r="H7" s="67">
+      <c r="H7" s="50">
         <f>((250*5)+(2*150)+(2*100))/100</f>
         <v>17.5</v>
       </c>
-      <c r="I7" s="68">
+      <c r="I7" s="51">
         <v>12</v>
       </c>
-      <c r="J7" s="70">
-        <f>C7*($F7/$M7)</f>
+      <c r="J7" s="53">
+        <f t="shared" ref="J7:L8" si="1">C7*($F7/$M7)</f>
         <v>7.2777394900068917E-2</v>
       </c>
-      <c r="K7" s="70">
-        <f>D7*($F7/$M7)</f>
+      <c r="K7" s="53">
+        <f t="shared" si="1"/>
         <v>1.0890925238172129</v>
       </c>
-      <c r="L7" s="70">
-        <f>E7*($F7/$M7)</f>
+      <c r="L7" s="53">
+        <f t="shared" si="1"/>
         <v>0.18183488345389828</v>
       </c>
-      <c r="M7" s="71">
+      <c r="M7" s="54">
         <f>F7+H7</f>
         <v>27.5</v>
       </c>
-      <c r="N7" s="83"/>
+      <c r="N7" s="61"/>
     </row>
     <row r="8" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B8" s="81">
+      <c r="B8" s="59">
         <v>7</v>
       </c>
-      <c r="C8" s="61">
+      <c r="C8" s="44">
         <f>'Stock Solutions'!$M$4</f>
         <v>0.2001378359751895</v>
       </c>
-      <c r="D8" s="62">
+      <c r="D8" s="45">
         <f>'Stock Solutions'!$O$4</f>
         <v>2.9950044404973353</v>
       </c>
-      <c r="E8" s="62">
+      <c r="E8" s="45">
         <f>'Stock Solutions'!$N$4</f>
         <v>0.50004592949822024</v>
       </c>
@@ -3413,27 +3448,27 @@
       <c r="I8" s="38">
         <v>12</v>
       </c>
-      <c r="J8" s="63">
-        <f>C8*($F8/$M8)</f>
+      <c r="J8" s="46">
+        <f t="shared" si="1"/>
         <v>6.8046864231564433E-2</v>
       </c>
-      <c r="K8" s="63">
-        <f>D8*($F8/$M8)</f>
+      <c r="K8" s="46">
+        <f t="shared" si="1"/>
         <v>1.0183015097690942</v>
       </c>
-      <c r="L8" s="63">
-        <f>E8*($F8/$M8)</f>
+      <c r="L8" s="46">
+        <f t="shared" si="1"/>
         <v>0.17001561602939488</v>
       </c>
-      <c r="M8" s="64">
+      <c r="M8" s="47">
         <v>50</v>
       </c>
-      <c r="N8" s="82">
+      <c r="N8" s="60">
         <v>43006</v>
       </c>
     </row>
     <row r="9" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B9" s="84"/>
+      <c r="B9" s="62"/>
       <c r="C9" s="38"/>
       <c r="D9" s="39"/>
       <c r="F9" s="40"/>
@@ -3442,11 +3477,11 @@
       <c r="I9" s="38"/>
       <c r="J9" s="39"/>
       <c r="K9" s="39"/>
-      <c r="M9" s="69"/>
-      <c r="N9" s="85"/>
+      <c r="M9" s="52"/>
+      <c r="N9" s="63"/>
     </row>
     <row r="10" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B10" s="81"/>
+      <c r="B10" s="59"/>
       <c r="C10" s="38"/>
       <c r="D10" s="39"/>
       <c r="F10" s="40"/>
@@ -3455,11 +3490,11 @@
       <c r="I10" s="38"/>
       <c r="J10" s="39"/>
       <c r="K10" s="39"/>
-      <c r="M10" s="69"/>
-      <c r="N10" s="85"/>
+      <c r="M10" s="52"/>
+      <c r="N10" s="63"/>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B11" s="81"/>
+      <c r="B11" s="59"/>
       <c r="C11" s="38"/>
       <c r="D11" s="39"/>
       <c r="F11" s="40"/>
@@ -3468,23 +3503,23 @@
       <c r="I11" s="38"/>
       <c r="J11" s="39"/>
       <c r="K11" s="39"/>
-      <c r="M11" s="69"/>
-      <c r="N11" s="85"/>
+      <c r="M11" s="52"/>
+      <c r="N11" s="63"/>
     </row>
     <row r="12" spans="2:14" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="86"/>
-      <c r="C12" s="87"/>
-      <c r="D12" s="88"/>
-      <c r="E12" s="88"/>
-      <c r="F12" s="89"/>
-      <c r="G12" s="87"/>
-      <c r="H12" s="89"/>
-      <c r="I12" s="87"/>
-      <c r="J12" s="88"/>
-      <c r="K12" s="88"/>
-      <c r="L12" s="90"/>
-      <c r="M12" s="91"/>
-      <c r="N12" s="92"/>
+      <c r="B12" s="64"/>
+      <c r="C12" s="65"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="67"/>
+      <c r="G12" s="65"/>
+      <c r="H12" s="67"/>
+      <c r="I12" s="65"/>
+      <c r="J12" s="66"/>
+      <c r="K12" s="66"/>
+      <c r="L12" s="68"/>
+      <c r="M12" s="69"/>
+      <c r="N12" s="70"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -3526,44 +3561,44 @@
   <sheetData>
     <row r="1" spans="1:19" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:19" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="47" t="s">
+      <c r="B2" s="132" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="134" t="s">
         <v>70</v>
       </c>
-      <c r="D2" s="51" t="s">
+      <c r="D2" s="136" t="s">
         <v>71</v>
       </c>
-      <c r="E2" s="52"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="54" t="s">
+      <c r="E2" s="137"/>
+      <c r="F2" s="138"/>
+      <c r="G2" s="139" t="s">
         <v>69</v>
       </c>
-      <c r="H2" s="55"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="54" t="s">
+      <c r="H2" s="140"/>
+      <c r="I2" s="134"/>
+      <c r="J2" s="139" t="s">
         <v>73</v>
       </c>
-      <c r="K2" s="55"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="51" t="s">
+      <c r="K2" s="140"/>
+      <c r="L2" s="134"/>
+      <c r="M2" s="136" t="s">
         <v>72</v>
       </c>
-      <c r="N2" s="52"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="51" t="s">
+      <c r="N2" s="137"/>
+      <c r="O2" s="138"/>
+      <c r="P2" s="136" t="s">
         <v>77</v>
       </c>
-      <c r="Q2" s="52"/>
-      <c r="R2" s="53"/>
+      <c r="Q2" s="137"/>
+      <c r="R2" s="138"/>
       <c r="S2" s="35" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:19" s="22" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="B3" s="48"/>
-      <c r="C3" s="50"/>
+      <c r="B3" s="133"/>
+      <c r="C3" s="135"/>
       <c r="D3" s="30" t="s">
         <v>66</v>
       </c>

</xml_diff>